<commit_message>
Demo relative range & describe current differences between Part Time & Full Time pay
</commit_message>
<xml_diff>
--- a/Interpreting Descriptive Statistics/Lesson Workbook 3 - Interpreting basic descriptive statistics.xlsx
+++ b/Interpreting Descriptive Statistics/Lesson Workbook 3 - Interpreting basic descriptive statistics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demai\Documents\Course Build\Workbooks\Module 1\1.2.4 Interpreting Basic Descriptive statistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sites\Data_Foundations_WithYouWithMe\Interpreting Descriptive Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBC266E-4BC9-495D-9B15-12C9AA869D12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8706709D-0270-45E6-BA6D-3303F019FE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="810" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{682ECE72-A850-4EEA-BAD4-BC6FFFC5916E}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="24690" windowHeight="14805" activeTab="3" xr2:uid="{682ECE72-A850-4EEA-BAD4-BC6FFFC5916E}"/>
   </bookViews>
   <sheets>
     <sheet name="Objectives" sheetId="3" r:id="rId1"/>
@@ -19,25 +19,19 @@
     <sheet name="Observations" sheetId="14" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Data-SanFranAccnt'!$A$1:$H$249</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Data-SanFranAccnt'!$H$1:$H$249</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="310">
   <si>
     <t>Benefits</t>
   </si>
@@ -982,9 +976,6 @@
     <t>Exercise Workbook 3</t>
   </si>
   <si>
-    <t>Basepay</t>
-  </si>
-  <si>
     <t>Average and Median values are similar. The large range in base pay, benefits and total pay suggest a large spread. Mode indicates possible skewness towards smaller values.</t>
   </si>
   <si>
@@ -993,6 +984,9 @@
   </si>
   <si>
     <t>Lesson - Interpreting basic descriptive statistics</t>
+  </si>
+  <si>
+    <t>Relative Range</t>
   </si>
 </sst>
 </file>
@@ -1000,10 +994,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1065,13 +1059,6 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1206,9 +1193,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1220,7 +1207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1230,7 +1217,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1239,7 +1226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -1254,99 +1241,92 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="3" builtinId="4"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1364,7 +1344,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1644,7 +1624,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1934,7 +1914,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2901,7 +2881,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="2:7" ht="9.9499999999999993" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -3058,138 +3038,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>292</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="27">
+      <c r="A2" s="26">
         <v>3087</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="27">
+      <c r="A3" s="26">
         <v>10768.338666666667</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="27">
+      <c r="A4" s="26">
         <v>18449.677333333333</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="27">
+      <c r="A5" s="26">
         <v>26131.016</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="27">
+      <c r="A6" s="26">
         <v>33812.354666666666</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="27">
+      <c r="A7" s="26">
         <v>41493.693333333329</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="27">
+      <c r="A8" s="26">
         <v>49175.031999999999</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="27">
+      <c r="A9" s="26">
         <v>56856.370666666669</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="27">
+      <c r="A10" s="26">
         <v>64537.709333333332</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="27">
+      <c r="A11" s="26">
         <v>72219.047999999995</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="27">
+      <c r="A12" s="26">
         <v>79900.386666666658</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12">
         <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="27">
+      <c r="A13" s="26">
         <v>87581.725333333336</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="27">
+      <c r="A14" s="26">
         <v>95263.063999999998</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14">
         <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="27">
+      <c r="A15" s="26">
         <v>102944.40266666666</v>
       </c>
-      <c r="B15" s="20">
+      <c r="B15">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="27">
+      <c r="A16" s="26">
         <v>110625.74133333334</v>
       </c>
-      <c r="B16" s="20">
+      <c r="B16">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="20" t="s">
         <v>293</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="20">
         <v>8</v>
       </c>
     </row>
@@ -3201,26 +3181,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5AD35FB-D9AE-40D2-BBF3-2FC1C7F5B683}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:H249"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A235" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D199" sqref="D199:D249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="14" style="13" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="14" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3250,7 +3230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>117889</v>
       </c>
@@ -3276,7 +3256,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>117890</v>
       </c>
@@ -3302,7 +3282,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>118056</v>
       </c>
@@ -3328,7 +3308,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>118334</v>
       </c>
@@ -3354,7 +3334,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>118762</v>
       </c>
@@ -3380,7 +3360,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>118761</v>
       </c>
@@ -3406,7 +3386,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>118763</v>
       </c>
@@ -3432,7 +3412,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>119253</v>
       </c>
@@ -3458,7 +3438,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>119352</v>
       </c>
@@ -3484,7 +3464,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>119380</v>
       </c>
@@ -3510,7 +3490,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>119381</v>
       </c>
@@ -3536,7 +3516,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>119383</v>
       </c>
@@ -3562,7 +3542,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>119385</v>
       </c>
@@ -3588,7 +3568,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>119386</v>
       </c>
@@ -3614,7 +3594,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>119387</v>
       </c>
@@ -3640,7 +3620,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>119388</v>
       </c>
@@ -3666,7 +3646,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>119392</v>
       </c>
@@ -3692,7 +3672,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>119391</v>
       </c>
@@ -3718,7 +3698,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>119390</v>
       </c>
@@ -3744,7 +3724,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>119389</v>
       </c>
@@ -3770,7 +3750,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>119394</v>
       </c>
@@ -3796,7 +3776,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>119393</v>
       </c>
@@ -3822,7 +3802,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>119401</v>
       </c>
@@ -3848,7 +3828,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>119400</v>
       </c>
@@ -3874,7 +3854,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>119399</v>
       </c>
@@ -3900,7 +3880,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>119398</v>
       </c>
@@ -3926,7 +3906,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>119397</v>
       </c>
@@ -3952,7 +3932,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>119396</v>
       </c>
@@ -3978,7 +3958,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>119395</v>
       </c>
@@ -4004,7 +3984,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>119402</v>
       </c>
@@ -4030,7 +4010,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>119403</v>
       </c>
@@ -4056,7 +4036,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>119603</v>
       </c>
@@ -4082,7 +4062,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>119781</v>
       </c>
@@ -4108,7 +4088,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>119823</v>
       </c>
@@ -4134,7 +4114,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12">
         <v>119957</v>
       </c>
@@ -4160,7 +4140,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <v>120364</v>
       </c>
@@ -4186,7 +4166,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>120440</v>
       </c>
@@ -4212,7 +4192,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>120667</v>
       </c>
@@ -4238,7 +4218,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <v>120781</v>
       </c>
@@ -4264,7 +4244,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <v>120783</v>
       </c>
@@ -4290,7 +4270,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <v>120850</v>
       </c>
@@ -4316,7 +4296,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <v>120851</v>
       </c>
@@ -4342,7 +4322,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <v>121082</v>
       </c>
@@ -4368,7 +4348,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <v>121310</v>
       </c>
@@ -4394,7 +4374,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <v>121311</v>
       </c>
@@ -4420,7 +4400,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <v>121479</v>
       </c>
@@ -4446,7 +4426,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>121697</v>
       </c>
@@ -4472,7 +4452,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>121918</v>
       </c>
@@ -4498,7 +4478,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12">
         <v>122002</v>
       </c>
@@ -4524,7 +4504,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12">
         <v>122011</v>
       </c>
@@ -4550,7 +4530,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12">
         <v>122313</v>
       </c>
@@ -4576,7 +4556,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12">
         <v>122315</v>
       </c>
@@ -4602,7 +4582,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12">
         <v>122083</v>
       </c>
@@ -4628,7 +4608,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12">
         <v>122262</v>
       </c>
@@ -4654,7 +4634,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12">
         <v>122322</v>
       </c>
@@ -4680,7 +4660,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12">
         <v>122505</v>
       </c>
@@ -4706,7 +4686,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="12">
         <v>122506</v>
       </c>
@@ -4732,7 +4712,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12">
         <v>122508</v>
       </c>
@@ -4758,7 +4738,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12">
         <v>122509</v>
       </c>
@@ -4784,7 +4764,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12">
         <v>122511</v>
       </c>
@@ -4810,7 +4790,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12">
         <v>122513</v>
       </c>
@@ -4836,7 +4816,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12">
         <v>122512</v>
       </c>
@@ -4862,7 +4842,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12">
         <v>122516</v>
       </c>
@@ -4888,7 +4868,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12">
         <v>122515</v>
       </c>
@@ -4914,7 +4894,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12">
         <v>122514</v>
       </c>
@@ -4940,7 +4920,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12">
         <v>122525</v>
       </c>
@@ -4966,7 +4946,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12">
         <v>122524</v>
       </c>
@@ -4992,7 +4972,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12">
         <v>122523</v>
       </c>
@@ -5018,7 +4998,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12">
         <v>122522</v>
       </c>
@@ -5044,7 +5024,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12">
         <v>122521</v>
       </c>
@@ -5070,7 +5050,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12">
         <v>122519</v>
       </c>
@@ -5096,7 +5076,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12">
         <v>122533</v>
       </c>
@@ -5122,7 +5102,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12">
         <v>122532</v>
       </c>
@@ -5148,7 +5128,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12">
         <v>122529</v>
       </c>
@@ -5174,7 +5154,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12">
         <v>122528</v>
       </c>
@@ -5200,7 +5180,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12">
         <v>122527</v>
       </c>
@@ -5226,7 +5206,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12">
         <v>122526</v>
       </c>
@@ -5252,7 +5232,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12">
         <v>122542</v>
       </c>
@@ -5278,7 +5258,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12">
         <v>122541</v>
       </c>
@@ -5304,7 +5284,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12">
         <v>122540</v>
       </c>
@@ -5330,7 +5310,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12">
         <v>122539</v>
       </c>
@@ -5356,7 +5336,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12">
         <v>122538</v>
       </c>
@@ -5382,7 +5362,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12">
         <v>122537</v>
       </c>
@@ -5408,7 +5388,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12">
         <v>122536</v>
       </c>
@@ -5434,7 +5414,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12">
         <v>122535</v>
       </c>
@@ -5460,7 +5440,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12">
         <v>122534</v>
       </c>
@@ -5486,7 +5466,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12">
         <v>122543</v>
       </c>
@@ -5512,7 +5492,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12">
         <v>122544</v>
       </c>
@@ -5538,7 +5518,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12">
         <v>122555</v>
       </c>
@@ -5564,7 +5544,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12">
         <v>122733</v>
       </c>
@@ -5590,7 +5570,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12">
         <v>122751</v>
       </c>
@@ -5616,7 +5596,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12">
         <v>122885</v>
       </c>
@@ -5642,7 +5622,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12">
         <v>122892</v>
       </c>
@@ -5668,7 +5648,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12">
         <v>122927</v>
       </c>
@@ -5694,7 +5674,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="12">
         <v>123388</v>
       </c>
@@ -5720,7 +5700,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12">
         <v>123516</v>
       </c>
@@ -5746,7 +5726,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="12">
         <v>123544</v>
       </c>
@@ -5772,7 +5752,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12">
         <v>123712</v>
       </c>
@@ -5798,7 +5778,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="12">
         <v>123713</v>
       </c>
@@ -5824,7 +5804,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="12">
         <v>124000</v>
       </c>
@@ -5850,7 +5830,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="12">
         <v>124015</v>
       </c>
@@ -5876,7 +5856,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="12">
         <v>124095</v>
       </c>
@@ -5902,7 +5882,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="12">
         <v>124706</v>
       </c>
@@ -5928,7 +5908,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="12">
         <v>124870</v>
       </c>
@@ -5954,7 +5934,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12">
         <v>125114</v>
       </c>
@@ -5980,7 +5960,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="12">
         <v>125255</v>
       </c>
@@ -6006,7 +5986,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="12">
         <v>125524</v>
       </c>
@@ -6032,7 +6012,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="12">
         <v>125567</v>
       </c>
@@ -6058,7 +6038,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="12">
         <v>125612</v>
       </c>
@@ -6084,7 +6064,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="12">
         <v>125684</v>
       </c>
@@ -6110,7 +6090,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="12">
         <v>125837</v>
       </c>
@@ -6136,7 +6116,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="12">
         <v>125857</v>
       </c>
@@ -6162,7 +6142,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="12">
         <v>125904</v>
       </c>
@@ -6188,7 +6168,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="12">
         <v>126000</v>
       </c>
@@ -6214,7 +6194,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="12">
         <v>126083</v>
       </c>
@@ -6240,7 +6220,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="12">
         <v>126125</v>
       </c>
@@ -6266,7 +6246,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="12">
         <v>126423</v>
       </c>
@@ -6292,7 +6272,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="12">
         <v>126427</v>
       </c>
@@ -6318,7 +6298,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="12">
         <v>126452</v>
       </c>
@@ -6344,7 +6324,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="12">
         <v>126806</v>
       </c>
@@ -6370,7 +6350,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="12">
         <v>126809</v>
       </c>
@@ -6396,7 +6376,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="12">
         <v>126836</v>
       </c>
@@ -6422,7 +6402,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="12">
         <v>127046</v>
       </c>
@@ -6448,7 +6428,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="12">
         <v>127048</v>
       </c>
@@ -6474,7 +6454,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="12">
         <v>127049</v>
       </c>
@@ -6500,7 +6480,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="12">
         <v>127050</v>
       </c>
@@ -6526,7 +6506,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="12">
         <v>127053</v>
       </c>
@@ -6552,7 +6532,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="12">
         <v>127052</v>
       </c>
@@ -6578,7 +6558,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="12">
         <v>127051</v>
       </c>
@@ -6604,7 +6584,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="12">
         <v>127054</v>
       </c>
@@ -6630,7 +6610,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="12">
         <v>127056</v>
       </c>
@@ -6656,7 +6636,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="12">
         <v>127055</v>
       </c>
@@ -6682,7 +6662,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="12">
         <v>127058</v>
       </c>
@@ -6708,7 +6688,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="12">
         <v>127057</v>
       </c>
@@ -6734,7 +6714,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="12">
         <v>127065</v>
       </c>
@@ -6760,7 +6740,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="12">
         <v>127063</v>
       </c>
@@ -6786,7 +6766,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="12">
         <v>127061</v>
       </c>
@@ -6812,7 +6792,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="12">
         <v>127060</v>
       </c>
@@ -6838,7 +6818,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="12">
         <v>127066</v>
       </c>
@@ -6864,7 +6844,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="12">
         <v>127064</v>
       </c>
@@ -6890,7 +6870,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="12">
         <v>127062</v>
       </c>
@@ -6916,7 +6896,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="12">
         <v>127069</v>
       </c>
@@ -6942,7 +6922,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="12">
         <v>127068</v>
       </c>
@@ -6968,7 +6948,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="12">
         <v>127067</v>
       </c>
@@ -6994,7 +6974,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="12">
         <v>127072</v>
       </c>
@@ -7020,7 +7000,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="12">
         <v>127070</v>
       </c>
@@ -7046,7 +7026,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="12">
         <v>127093</v>
       </c>
@@ -7072,7 +7052,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="149" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="12">
         <v>127156</v>
       </c>
@@ -7098,7 +7078,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="150" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="12">
         <v>127260</v>
       </c>
@@ -7124,7 +7104,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="151" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="12">
         <v>127467</v>
       </c>
@@ -7150,7 +7130,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="152" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="12">
         <v>127960</v>
       </c>
@@ -7176,7 +7156,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="153" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="12">
         <v>128070</v>
       </c>
@@ -7202,7 +7182,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="154" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="12">
         <v>128071</v>
       </c>
@@ -7228,7 +7208,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="155" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="12">
         <v>128298</v>
       </c>
@@ -7254,7 +7234,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="156" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="12">
         <v>128455</v>
       </c>
@@ -7280,7 +7260,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="12">
         <v>128507</v>
       </c>
@@ -7306,7 +7286,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="158" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="12">
         <v>128673</v>
       </c>
@@ -7332,7 +7312,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="159" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="12">
         <v>129182</v>
       </c>
@@ -7358,7 +7338,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="160" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="12">
         <v>129186</v>
       </c>
@@ -7384,7 +7364,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="161" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="12">
         <v>129187</v>
       </c>
@@ -7410,7 +7390,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="162" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="12">
         <v>129252</v>
       </c>
@@ -7436,7 +7416,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="163" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="12">
         <v>129375</v>
       </c>
@@ -7462,7 +7442,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="164" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="12">
         <v>129873</v>
       </c>
@@ -7488,7 +7468,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="165" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="12">
         <v>130536</v>
       </c>
@@ -7514,7 +7494,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="166" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="12">
         <v>130806</v>
       </c>
@@ -7540,7 +7520,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="167" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="12">
         <v>130807</v>
       </c>
@@ -7566,7 +7546,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="12">
         <v>130809</v>
       </c>
@@ -7592,7 +7572,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="169" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="12">
         <v>130808</v>
       </c>
@@ -7618,7 +7598,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="12">
         <v>130812</v>
       </c>
@@ -7644,7 +7624,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="12">
         <v>130811</v>
       </c>
@@ -7670,7 +7650,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="172" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="12">
         <v>130810</v>
       </c>
@@ -7696,7 +7676,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="12">
         <v>130814</v>
       </c>
@@ -7722,7 +7702,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="174" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="12">
         <v>130813</v>
       </c>
@@ -7748,7 +7728,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="175" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="12">
         <v>130817</v>
       </c>
@@ -7774,7 +7754,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="176" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="12">
         <v>130819</v>
       </c>
@@ -7800,7 +7780,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="177" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="12">
         <v>130818</v>
       </c>
@@ -7826,7 +7806,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="178" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="12">
         <v>130860</v>
       </c>
@@ -7852,7 +7832,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="179" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="12">
         <v>130979</v>
       </c>
@@ -7878,7 +7858,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="180" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="12">
         <v>130990</v>
       </c>
@@ -7904,7 +7884,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="181" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12">
         <v>131514</v>
       </c>
@@ -7930,7 +7910,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="12">
         <v>131792</v>
       </c>
@@ -7956,7 +7936,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="12">
         <v>131845</v>
       </c>
@@ -7982,7 +7962,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="12">
         <v>132587</v>
       </c>
@@ -8008,7 +7988,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="12">
         <v>132606</v>
       </c>
@@ -8034,7 +8014,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="12">
         <v>132682</v>
       </c>
@@ -8060,7 +8040,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="12">
         <v>132683</v>
       </c>
@@ -8086,7 +8066,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="188" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="12">
         <v>132684</v>
       </c>
@@ -8112,7 +8092,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="189" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="12">
         <v>132686</v>
       </c>
@@ -8138,7 +8118,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="190" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="12">
         <v>132685</v>
       </c>
@@ -8164,7 +8144,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="191" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="12">
         <v>132688</v>
       </c>
@@ -8190,7 +8170,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="192" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="12">
         <v>132705</v>
       </c>
@@ -8216,7 +8196,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="193" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="12">
         <v>132741</v>
       </c>
@@ -8242,7 +8222,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="194" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="12">
         <v>133304</v>
       </c>
@@ -8268,7 +8248,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="195" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="12">
         <v>133619</v>
       </c>
@@ -8294,7 +8274,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="196" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="12">
         <v>133620</v>
       </c>
@@ -8320,7 +8300,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="197" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="12">
         <v>133842</v>
       </c>
@@ -8346,7 +8326,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="198" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" ht="24.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="12">
         <v>136181</v>
       </c>
@@ -9699,6 +9679,16 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="H1:H249" xr:uid="{E5AD35FB-D9AE-40D2-BBF3-2FC1C7F5B683}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Part Time"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H249">
+      <sortCondition ref="H1:H249"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -9712,8 +9702,8 @@
   </sheetPr>
   <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9722,7 +9712,7 @@
     <col min="2" max="6" width="10.7109375" customWidth="1"/>
     <col min="7" max="7" width="6.42578125" customWidth="1"/>
     <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" customWidth="1"/>
     <col min="11" max="11" width="41.5703125" customWidth="1"/>
     <col min="12" max="18" width="5.7109375" customWidth="1"/>
@@ -9732,42 +9722,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="H1" s="36" t="s">
-        <v>306</v>
-      </c>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="H1" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
     </row>
     <row r="2" spans="1:24" s="13" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>273</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="27" t="s">
         <v>280</v>
       </c>
-      <c r="E2" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="24" t="s">
+      <c r="E2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="37" t="s">
+      <c r="H2" s="47" t="s">
         <v>273</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="I2" s="48" t="s">
         <v>302</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="J2" s="48" t="s">
         <v>271</v>
       </c>
+      <c r="K2" s="47"/>
       <c r="S2" s="15"/>
     </row>
     <row r="3" spans="1:24" s="13" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -9780,17 +9772,23 @@
       <c r="D3" s="19">
         <v>4.0502419354838706</v>
       </c>
-      <c r="E3" s="33">
+      <c r="E3" s="32">
         <v>28566.471209677456</v>
       </c>
-      <c r="F3" s="33">
+      <c r="F3" s="32">
         <v>106115.57028225798</v>
       </c>
-      <c r="H3" s="37" t="s">
+      <c r="H3" s="47" t="s">
         <v>274</v>
       </c>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="I3" s="14">
+        <f>AVERAGE('Data-SanFranAccnt'!D$2:D$198)</f>
+        <v>87646.048680203006</v>
+      </c>
+      <c r="J3" s="14">
+        <f>AVERAGE('Data-SanFranAccnt'!D$199:D$249)</f>
+        <v>38527.461176470584</v>
+      </c>
       <c r="K3" s="15"/>
       <c r="L3" s="15"/>
       <c r="M3" s="15"/>
@@ -9815,17 +9813,24 @@
       <c r="D4" s="19">
         <v>0</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="32">
         <v>31076.85</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="32">
         <v>109876.15</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="47" t="s">
         <v>275</v>
       </c>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
+      <c r="I4" s="14">
+        <f>MEDIAN('Data-SanFranAccnt'!D$2:D$198)</f>
+        <v>90290.73</v>
+      </c>
+      <c r="J4" s="14">
+        <f>MEDIAN('Data-SanFranAccnt'!D$199:D$249)</f>
+        <v>32971.269999999997</v>
+      </c>
+      <c r="K4" s="47"/>
       <c r="U4" s="14"/>
       <c r="V4" s="14"/>
       <c r="W4" s="14"/>
@@ -9834,23 +9839,30 @@
       <c r="B5" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="32">
         <v>94984</v>
       </c>
-      <c r="D5" s="33">
-        <v>0</v>
-      </c>
-      <c r="E5" s="33">
+      <c r="D5" s="32">
+        <v>0</v>
+      </c>
+      <c r="E5" s="32">
         <v>34621.43</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="32">
         <v>129605.43</v>
       </c>
-      <c r="H5" s="37" t="s">
+      <c r="H5" s="47" t="s">
         <v>276</v>
       </c>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
+      <c r="I5" s="14">
+        <f>MODE('Data-SanFranAccnt'!D$2:D$198)</f>
+        <v>94984</v>
+      </c>
+      <c r="J5" s="14">
+        <f>MODE('Data-SanFranAccnt'!D$199:D$249)</f>
+        <v>19729</v>
+      </c>
+      <c r="K5" s="47"/>
       <c r="U5" s="14"/>
       <c r="V5" s="14"/>
       <c r="W5" s="14"/>
@@ -9859,23 +9871,30 @@
       <c r="B6" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="C6" s="34">
+      <c r="C6" s="33">
         <v>118307.08</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="33">
         <v>620.54999999999995</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="33">
         <v>39134.639999999999</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="33">
         <v>157441.72</v>
       </c>
-      <c r="H6" s="37" t="s">
+      <c r="H6" s="47" t="s">
         <v>277</v>
       </c>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
+      <c r="I6" s="14">
+        <f>MAX('Data-SanFranAccnt'!D$2:D$198)</f>
+        <v>118307.08</v>
+      </c>
+      <c r="J6" s="14">
+        <f>MAX('Data-SanFranAccnt'!D$199:D$249)</f>
+        <v>90605.18</v>
+      </c>
+      <c r="K6" s="47"/>
       <c r="U6" s="14"/>
       <c r="V6" s="14"/>
       <c r="W6" s="14"/>
@@ -9884,23 +9903,30 @@
       <c r="B7" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="C7" s="34">
+      <c r="C7" s="33">
         <v>3087</v>
       </c>
-      <c r="D7" s="34">
-        <v>0</v>
-      </c>
-      <c r="E7" s="34">
-        <v>0</v>
-      </c>
-      <c r="F7" s="34">
+      <c r="D7" s="33">
+        <v>0</v>
+      </c>
+      <c r="E7" s="33">
+        <v>0</v>
+      </c>
+      <c r="F7" s="33">
         <v>3810.2799999999997</v>
       </c>
-      <c r="H7" s="37" t="s">
+      <c r="H7" s="47" t="s">
         <v>278</v>
       </c>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
+      <c r="I7" s="14">
+        <f>MIN('Data-SanFranAccnt'!D$2:D$198)</f>
+        <v>58671.65</v>
+      </c>
+      <c r="J7" s="14">
+        <f>MIN('Data-SanFranAccnt'!D$199:D$249)</f>
+        <v>3087</v>
+      </c>
+      <c r="K7" s="47"/>
       <c r="U7" s="14"/>
       <c r="V7" s="14"/>
       <c r="W7" s="14"/>
@@ -9909,43 +9935,59 @@
       <c r="B8" s="18" t="s">
         <v>279</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="32">
         <v>115220.08</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="32">
         <v>620.54999999999995</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="32">
         <v>39134.639999999999</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="32">
         <v>153631.44</v>
       </c>
       <c r="G8" s="15"/>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="47" t="s">
         <v>279</v>
       </c>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
+      <c r="I8" s="14">
+        <f>I6-I7</f>
+        <v>59635.43</v>
+      </c>
+      <c r="J8" s="14">
+        <f>J6-J7</f>
+        <v>87518.18</v>
+      </c>
+      <c r="K8" s="47"/>
       <c r="U8" s="14"/>
       <c r="V8" s="14"/>
       <c r="W8" s="14"/>
       <c r="X8" s="15"/>
     </row>
     <row r="9" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="47" t="s">
+        <v>309</v>
+      </c>
+      <c r="I9" s="22">
+        <f>I8/I3</f>
+        <v>0.68041207673370119</v>
+      </c>
+      <c r="J9" s="22">
+        <f>J8/J3</f>
+        <v>2.271579214605735</v>
+      </c>
+      <c r="K9" s="46"/>
       <c r="U9" s="7"/>
       <c r="V9" s="7"/>
       <c r="W9" s="7"/>
-      <c r="X9" s="23"/>
+      <c r="X9" s="22"/>
     </row>
     <row r="10" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="16"/>
@@ -9958,96 +10000,96 @@
       <c r="A11" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="34" t="s">
         <v>281</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43" t="s">
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34" t="s">
         <v>296</v>
       </c>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="26" t="s">
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="25" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="40">
+      <c r="A12" s="36">
         <v>1</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="37" t="s">
+        <v>306</v>
+      </c>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="40" t="s">
+        <v>299</v>
+      </c>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="42" t="s">
         <v>307</v>
       </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="51"/>
-      <c r="G12" s="44" t="s">
-        <v>299</v>
-      </c>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="41" t="s">
-        <v>308</v>
-      </c>
     </row>
     <row r="13" spans="1:24" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="40">
+      <c r="A13" s="36">
         <v>2</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="43" t="s">
         <v>297</v>
       </c>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="48" t="s">
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="44" t="s">
         <v>300</v>
       </c>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="42" t="s">
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="45" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="40">
+      <c r="A14" s="36">
         <v>3</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="43" t="s">
         <v>303</v>
       </c>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="41" t="s">
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="42" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="32"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="31"/>
     </row>
     <row r="16" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>

</xml_diff>